<commit_message>
Added encoder cad model and excel sheet with needed parts
</commit_message>
<xml_diff>
--- a/docs/parts.xlsx
+++ b/docs/parts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -40,6 +40,36 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>CHERRY MX 540-MX1A-E1NW</t>
+  </si>
+  <si>
+    <t>Mechanical pushbutton switch</t>
+  </si>
+  <si>
+    <t>WURTH ELEKTRONIK 482009514001</t>
+  </si>
+  <si>
+    <t>Mechanical incremental encoder with switch</t>
+  </si>
+  <si>
+    <t>cherry mx - mouser.com</t>
+  </si>
+  <si>
+    <t>wurth incremental encoder - mouser.com</t>
+  </si>
+  <si>
+    <t>LED RGB WS2812B RING</t>
+  </si>
+  <si>
+    <t>Ring of 8 RGB LED diodes</t>
+  </si>
+  <si>
+    <t>ws2812 RGB LED - botland.pl</t>
+  </si>
+  <si>
+    <t>STM32F401RCT - lcsc.com</t>
   </si>
 </sst>
 </file>
@@ -47,10 +77,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="#,##0.000\ [$USD]"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000\ [$USD]"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,8 +89,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -129,19 +167,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -423,7 +469,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,150 +478,207 @@
     <col min="2" max="2" width="79.77734375" customWidth="1"/>
     <col min="3" max="3" width="17.88671875" customWidth="1"/>
     <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="44.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>6.7226999999999997</v>
       </c>
+      <c r="E2" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="4"/>
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="4"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>